<commit_message>
XLS file with multiple options and menus
</commit_message>
<xml_diff>
--- a/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
+++ b/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KarolinaSedlackova\waw_t2c\example\mp3_app\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2FE1C4BB-DC25-43EC-B7B4-6A1D8C82B01E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F33B136-BF62-43F9-B5E7-24824CEE63A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11670" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>#E_L</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Toto je testovací dokument</t>
   </si>
   <si>
-    <t>V prvním sloupci jsou činnosti, na které se pak reaguje pravým sloupcem.</t>
-  </si>
-  <si>
     <t>Soubory v pravé části se převedou do mp3 souborů</t>
   </si>
   <si>
@@ -81,32 +78,65 @@
     <t>item12</t>
   </si>
   <si>
-    <t>Veličiny můţeme rozdělit i do intervalů, které si určíme</t>
-  </si>
-  <si>
-    <t>Poloha vlastně znamená, ţe pokud si představíme číselnou osu a chtěli by jsme na ni naznačit to hafo našich čísel (př. ty výšky dětí) jen jediným bodem, kam by jsme dali značku. Je to vlastně jaká si střední hodnota</t>
-  </si>
-  <si>
-    <t>Nás zajímá hlavně aritmetický – tzn. klasika, sčítám všechny hodnoty jsme naměřili a vydělím je počtem měření</t>
-  </si>
-  <si>
-    <t>Variabilita je vzdálenost našich naměřených hodnot od střední hodnoty</t>
-  </si>
-  <si>
-    <t>Kdyţ počítáme rozptyl tak od kaţdé naměřené hodnoty odečteme průměr všech naměřených hodnot</t>
-  </si>
-  <si>
     <t>!Menu Main_menu flat;order=last;timeout=1000</t>
   </si>
   <si>
     <t>!!Menu</t>
+  </si>
+  <si>
+    <t>V prvním sloupci jsou činnosti, na které se pak reaguje pravým sloupcem</t>
+  </si>
+  <si>
+    <t>!Menu Second_menu round;order=last;timeout=500</t>
+  </si>
+  <si>
+    <t>položka menu 21</t>
+  </si>
+  <si>
+    <t>položka menu 22</t>
+  </si>
+  <si>
+    <t>item3_handler</t>
+  </si>
+  <si>
+    <t>položka menu 31</t>
+  </si>
+  <si>
+    <t>položka menu 32</t>
+  </si>
+  <si>
+    <t>položka menu 33</t>
+  </si>
+  <si>
+    <t>item4_handler</t>
+  </si>
+  <si>
+    <t>položka menu 41</t>
+  </si>
+  <si>
+    <t>položka menu 42</t>
+  </si>
+  <si>
+    <t>item5_handler</t>
+  </si>
+  <si>
+    <t>položka menu 51</t>
+  </si>
+  <si>
+    <t>položka menu 52</t>
+  </si>
+  <si>
+    <t>item6_handler</t>
+  </si>
+  <si>
+    <t>!Menu Third_menu round;order=first;timeout=1000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,16 +146,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,13 +192,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,22 +515,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52629F32-2B48-4C6C-A705-AE46732F66E2}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="39.7265625" customWidth="1"/>
+    <col min="2" max="2" width="39.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -493,128 +539,187 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="28" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="25" x14ac:dyDescent="0.35">
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
+      <c r="B21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>16</v>
+      <c r="B28" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>17</v>
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>24</v>
+      <c r="B31" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B39" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B43" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding examples of actions, mapping intent-value and naming for reaction patterns
</commit_message>
<xml_diff>
--- a/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
+++ b/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KarolinaSedlackova\waw_t2c\example\mp3_app\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tom\Watson\public_workspaces\watson-assistant-workbench_mp3\example\mp3_app\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F33B136-BF62-43F9-B5E7-24824CEE63A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7117B6BB-BD11-4C4C-84E3-0B600F0F6615}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11670" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12336" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>#E_L</t>
   </si>
@@ -130,13 +131,64 @@
   </si>
   <si>
     <t>!Menu Third_menu round;order=first;timeout=1000</t>
+  </si>
+  <si>
+    <t>// This is example of the default reaction pattern as we do not specify any !Reaction here yet. The same effect wold have !Reaction default</t>
+  </si>
+  <si>
+    <t>!Reaction MyReactionSet1</t>
+  </si>
+  <si>
+    <t>!!MyReactionSet1</t>
+  </si>
+  <si>
+    <t>My local reaction to left</t>
+  </si>
+  <si>
+    <t>My local reaction to right</t>
+  </si>
+  <si>
+    <t>!Define #E_L = 1</t>
+  </si>
+  <si>
+    <t>!Define #E_R =2</t>
+  </si>
+  <si>
+    <t>!Define #E_Button1 =20</t>
+  </si>
+  <si>
+    <t>/// Intent names mapping to values (optional for standard events)</t>
+  </si>
+  <si>
+    <t>//  This is example of not standard event which must be added to the platform</t>
+  </si>
+  <si>
+    <t>/// Platform specific intents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!Action  litP2 =200  </t>
+  </si>
+  <si>
+    <t>!Action  litP1</t>
+  </si>
+  <si>
+    <t>/// Default reaction is overriden for two intents, the rest reminds to be handled by default</t>
+  </si>
+  <si>
+    <t>/// Definition of platform specific action.   (Mind: menu, or reactive patterns are also actions)</t>
+  </si>
+  <si>
+    <t>// This is definition of the action name, value is assigned automatically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Here we enforce also the value </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,12 +200,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -192,15 +238,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,210 +557,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52629F32-2B48-4C6C-A705-AE46732F66E2}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="28" x14ac:dyDescent="0.35">
-      <c r="B13" s="3" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="4" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="4" t="s">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C51" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="4" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="4" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C54" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="4" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="4" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="4" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C62" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="4" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="5" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="4"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="4" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C66" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="4" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>18</v>
       </c>
     </row>
@@ -726,4 +893,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43F3A0C-F00B-4F57-A836-9E5A5E11B589}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New version of xls file added
</commit_message>
<xml_diff>
--- a/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
+++ b/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tom\Watson\public_workspaces\watson-assistant-workbench_mp3\example\mp3_app\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KarolinaSedlackova\waw_t2c\example\mp3_app\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7117B6BB-BD11-4C4C-84E3-0B600F0F6615}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5C2B4A-C24B-4323-8201-9EAF0C90B6A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12336" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8390" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>#E_L</t>
   </si>
@@ -182,6 +182,21 @@
   </si>
   <si>
     <t xml:space="preserve">// Here we enforce also the value </t>
+  </si>
+  <si>
+    <t>!Define #E_U=3</t>
+  </si>
+  <si>
+    <t>!Define #E_D=4</t>
+  </si>
+  <si>
+    <t>!Folder 01</t>
+  </si>
+  <si>
+    <t>!!Folder</t>
+  </si>
+  <si>
+    <t>!Folder 02</t>
   </si>
 </sst>
 </file>
@@ -557,335 +572,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52629F32-2B48-4C6C-A705-AE46732F66E2}">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>49</v>
       </c>
-      <c r="B8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>47</v>
       </c>
-      <c r="B10"/>
-      <c r="C10" t="s">
+      <c r="B14"/>
+      <c r="C14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B12"/>
-      <c r="C12" t="s">
+      <c r="B16"/>
+      <c r="C16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B18"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B20"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B28"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B34"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="B29"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B30"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B31"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>0</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B33"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>1</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B45"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B47"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>37</v>
       </c>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="B48"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B37"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="2" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="2" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B53" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="2" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B54" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="2" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C56" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B63" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="2" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B70" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B71" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B74" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C74" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="2" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B75" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="3" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B76" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B78" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C78" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="2" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B79" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>18</v>
       </c>
     </row>
@@ -903,7 +951,7 @@
       <selection sqref="A1:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated example .xls to demonstrate actions
</commit_message>
<xml_diff>
--- a/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
+++ b/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KarolinaSedlackova\waw_t2c\example\mp3_app\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tom\Watson\public_workspaces\watson-assistant-workbench_mp3\example\mp3_app\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5C2B4A-C24B-4323-8201-9EAF0C90B6A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816AA8AB-6563-4D35-9D32-C78EF62CA567}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8390" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12336" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>#E_L</t>
   </si>
@@ -64,15 +64,9 @@
     <t>item1</t>
   </si>
   <si>
-    <t>item1_handler</t>
-  </si>
-  <si>
     <t>item2</t>
   </si>
   <si>
-    <t>item2_handler</t>
-  </si>
-  <si>
     <t>item11</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>položka menu 22</t>
   </si>
   <si>
-    <t>item3_handler</t>
-  </si>
-  <si>
     <t>položka menu 31</t>
   </si>
   <si>
@@ -109,27 +100,18 @@
     <t>položka menu 33</t>
   </si>
   <si>
-    <t>item4_handler</t>
-  </si>
-  <si>
     <t>položka menu 41</t>
   </si>
   <si>
     <t>položka menu 42</t>
   </si>
   <si>
-    <t>item5_handler</t>
-  </si>
-  <si>
     <t>položka menu 51</t>
   </si>
   <si>
     <t>položka menu 52</t>
   </si>
   <si>
-    <t>item6_handler</t>
-  </si>
-  <si>
     <t>!Menu Third_menu round;order=first;timeout=1000</t>
   </si>
   <si>
@@ -178,12 +160,6 @@
     <t>/// Definition of platform specific action.   (Mind: menu, or reactive patterns are also actions)</t>
   </si>
   <si>
-    <t>// This is definition of the action name, value is assigned automatically</t>
-  </si>
-  <si>
-    <t xml:space="preserve">// Here we enforce also the value </t>
-  </si>
-  <si>
     <t>!Define #E_U=3</t>
   </si>
   <si>
@@ -197,6 +173,72 @@
   </si>
   <si>
     <t>!Folder 02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// Here is action assigned to fixed value  </t>
+  </si>
+  <si>
+    <t>// This is definition of the action name, value is assigned automatically  (as it is first, it will be of velue 1)</t>
+  </si>
+  <si>
+    <t>// this creates action MyReactionSet1 and assignes valu automatically to 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// this creates action Main_menu and assignes it a value which is 3 </t>
+  </si>
+  <si>
+    <t>litP2</t>
+  </si>
+  <si>
+    <t>//value of action is 200</t>
+  </si>
+  <si>
+    <t>Second_menu</t>
+  </si>
+  <si>
+    <t>// this creates action Second_menu and assignes it a value which is 4</t>
+  </si>
+  <si>
+    <t>// the value of Second_menu is 4 - determined in first pass throu and assigned in second</t>
+  </si>
+  <si>
+    <t>Main_menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// the value of Main_menu is 3 </t>
+  </si>
+  <si>
+    <t>// this creates action Third_menu and assignes it a value which is 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!Action  litP3  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">!Action  litP4  </t>
+  </si>
+  <si>
+    <t>!Action  litP5</t>
+  </si>
+  <si>
+    <t>// litP5 is assigned automatically next value which is 6</t>
+  </si>
+  <si>
+    <t>// litP3 is assigned automatically next value which is 7</t>
+  </si>
+  <si>
+    <t>// litP4 is assigned automatically next value which is 8</t>
+  </si>
+  <si>
+    <t>litP4</t>
+  </si>
+  <si>
+    <t>litP5</t>
+  </si>
+  <si>
+    <t>//value of action is 8</t>
+  </si>
+  <si>
+    <t>//value of action is 6</t>
   </si>
 </sst>
 </file>
@@ -572,91 +614,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52629F32-2B48-4C6C-A705-AE46732F66E2}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>47</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -664,21 +706,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -686,10 +728,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -697,10 +739,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B28"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -708,10 +750,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -719,222 +761,276 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B35"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B37"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B38"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B40"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B48"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C52" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="2" t="s">
+      <c r="C56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="B60" s="2"/>
+      <c r="C60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="2" t="s">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C69" t="s">
+        <v>67</v>
+      </c>
+      <c r="E69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B63" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>18</v>
-      </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B69" s="2" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C74" t="s">
+        <v>68</v>
+      </c>
+      <c r="E74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B76" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B78" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C74" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B76" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C78" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B79" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +1047,7 @@
       <selection sqref="A1:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
XLSX file edited, added folders to menu
</commit_message>
<xml_diff>
--- a/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
+++ b/example/mp3_app/xls/Watson_assistant_mp3_extensionCZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tom\Watson\public_workspaces\watson-assistant-workbench_mp3\example\mp3_app\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KarolinaSedlackova\waw_t2c\example\mp3_app\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816AA8AB-6563-4D35-9D32-C78EF62CA567}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CAA313-83E4-4229-8024-0D66BA3CD684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12336" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12340" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="74">
   <si>
     <t>#E_L</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>//value of action is 6</t>
+  </si>
+  <si>
+    <t>!Folder 03</t>
+  </si>
+  <si>
+    <t>!Folder 04</t>
+  </si>
+  <si>
+    <t>!Folder 05</t>
   </si>
 </sst>
 </file>
@@ -614,43 +623,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52629F32-2B48-4C6C-A705-AE46732F66E2}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -658,16 +667,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>43</v>
       </c>
       <c r="B12"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -676,7 +685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -685,20 +694,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B17"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -706,10 +715,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -717,10 +726,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B24"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -728,10 +737,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B26"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -739,10 +748,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B28"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -750,10 +759,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B30"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -761,35 +770,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B34"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>47</v>
       </c>
       <c r="B35"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B36"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>39</v>
       </c>
       <c r="B37"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -798,16 +807,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B39"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
       <c r="B40"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -815,7 +824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -823,213 +832,267 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B45"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>47</v>
       </c>
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>31</v>
       </c>
       <c r="B48"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B51"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>15</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C55" t="s">
         <v>53</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="2" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B56" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="2" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C59" t="s">
         <v>55</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="2"/>
-      <c r="C60" t="s">
+      <c r="B67" s="2"/>
+      <c r="C67" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="2" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B69" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C69" t="s">
         <v>58</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E69" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="2" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B70" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>28</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C78" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B69" s="2" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B80" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C80" t="s">
         <v>67</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E80" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B70" s="2" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B81" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B71" s="2" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B82" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B74" s="2" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B85" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C85" t="s">
         <v>68</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E85" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B75" s="2" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B86" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B76" s="3" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B87" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B78" s="2" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B89" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C89" t="s">
         <v>67</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E89" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B79" s="2" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B90" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>63</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C96" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>61</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C98" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>62</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C100" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1047,7 +1110,7 @@
       <selection sqref="A1:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>